<commit_message>
new cleaned data set
</commit_message>
<xml_diff>
--- a/Cleaned_data.xlsx
+++ b/Cleaned_data.xlsx
@@ -1,25 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\demo_fin\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD9E433-EF6B-44E1-AC36-ADE10194C31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8180"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demo" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -687,22 +701,19 @@
     <t>House for sale</t>
   </si>
   <si>
-    <t>2,121390 FWR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">565,680,,000 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">353,550,,000 </t>
+    <t>status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$RWF]\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="169" formatCode="_-[$RWF]\ * #,##0.00_-;\-[$RWF]\ * #,##0.00_-;_-[$RWF]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1139,7 +1150,7 @@
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1182,9 +1193,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1506,24 +1520,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F224"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="73.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
@@ -1532,15 +1547,18 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>300000000</v>
       </c>
       <c r="D2">
@@ -1562,14 +1580,14 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>300000000</v>
       </c>
       <c r="D3">
@@ -1579,14 +1597,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>450000000</v>
       </c>
       <c r="D4">
@@ -1596,14 +1614,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>155562000</v>
       </c>
       <c r="D5">
@@ -1613,14 +1631,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>160000000</v>
       </c>
       <c r="D6">
@@ -1630,14 +1648,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>165000000</v>
       </c>
       <c r="D7">
@@ -1647,14 +1665,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>450000000</v>
       </c>
       <c r="D8">
@@ -1664,14 +1682,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>45000000</v>
       </c>
       <c r="D9">
@@ -1681,14 +1699,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>250000000</v>
       </c>
       <c r="D10">
@@ -1698,14 +1716,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>100000000</v>
       </c>
       <c r="D11">
@@ -1715,15 +1733,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>71</v>
+      <c r="C12" s="1">
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1731,16 +1749,19 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F12" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>223</v>
+      <c r="C13" s="4">
+        <v>565680000</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1749,14 +1770,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <v>260000000</v>
       </c>
       <c r="D14">
@@ -1766,14 +1787,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <v>250000000</v>
       </c>
       <c r="D15">
@@ -1783,14 +1804,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <v>200000000</v>
       </c>
       <c r="D16">
@@ -1800,14 +1821,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <v>34000000</v>
       </c>
       <c r="D17">
@@ -1817,14 +1838,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <v>300000000</v>
       </c>
       <c r="D18">
@@ -1834,14 +1855,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="4">
         <v>300000000</v>
       </c>
       <c r="D19">
@@ -1851,14 +1872,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="4">
         <v>395976000</v>
       </c>
       <c r="D20">
@@ -1868,14 +1889,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="4">
         <v>200000000</v>
       </c>
       <c r="D21">
@@ -1885,14 +1906,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="4">
         <v>350000000</v>
       </c>
       <c r="D22">
@@ -1902,14 +1923,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="4">
         <v>300000000</v>
       </c>
       <c r="D23">
@@ -1919,11 +1940,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="4">
         <v>3000000</v>
       </c>
       <c r="D24">
@@ -1933,14 +1954,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="4">
         <v>170000000</v>
       </c>
       <c r="D25">
@@ -1950,14 +1971,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="4">
         <v>165000000</v>
       </c>
       <c r="D26">
@@ -1967,14 +1988,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="4">
         <v>300000000</v>
       </c>
       <c r="D27">
@@ -1984,14 +2005,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="4">
         <v>300000000</v>
       </c>
       <c r="D28">
@@ -2001,14 +2022,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="4">
         <v>353550000</v>
       </c>
       <c r="D29">
@@ -2018,11 +2039,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="4">
         <v>395976000</v>
       </c>
       <c r="D30">
@@ -2032,14 +2053,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="4">
         <v>250000000</v>
       </c>
       <c r="D31">
@@ -2049,14 +2070,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="4">
         <v>500000000</v>
       </c>
       <c r="D32">
@@ -2066,14 +2087,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="4">
         <v>180000000</v>
       </c>
       <c r="D33">
@@ -2083,14 +2104,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="4">
         <v>350000000</v>
       </c>
       <c r="D34">
@@ -2100,15 +2121,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>224</v>
+      <c r="C35" s="4">
+        <v>353550000</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2117,14 +2138,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="4">
         <v>70000000</v>
       </c>
       <c r="D36">
@@ -2134,14 +2155,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="4">
         <v>250000000</v>
       </c>
       <c r="D37">
@@ -2151,14 +2172,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="4">
         <v>180000000</v>
       </c>
       <c r="D38">
@@ -2168,14 +2189,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="4">
         <v>523254000</v>
       </c>
       <c r="D39">
@@ -2185,14 +2206,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="4">
         <v>155562000</v>
       </c>
       <c r="D40">
@@ -2202,14 +2223,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="4">
         <v>68000000</v>
       </c>
       <c r="D41">
@@ -2219,14 +2240,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="4">
         <v>270000000</v>
       </c>
       <c r="D42">
@@ -2236,14 +2257,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="4">
         <v>350000000</v>
       </c>
       <c r="D43">
@@ -2253,14 +2274,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="4">
         <v>280000000</v>
       </c>
       <c r="D44">
@@ -2270,14 +2291,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="4">
         <v>30000000</v>
       </c>
       <c r="D45">
@@ -2287,14 +2308,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="4">
         <v>1000000000</v>
       </c>
       <c r="D46">
@@ -2304,14 +2325,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="4">
         <v>2121300000</v>
       </c>
       <c r="D47">
@@ -2321,14 +2342,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="4">
         <v>38000000</v>
       </c>
       <c r="D48">
@@ -2338,14 +2359,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="4">
         <v>150000000</v>
       </c>
       <c r="D49">
@@ -2355,14 +2376,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="4">
         <v>280000000</v>
       </c>
       <c r="D50">
@@ -2372,14 +2393,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="4">
         <v>500000000</v>
       </c>
       <c r="D51">
@@ -2389,14 +2410,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="4">
         <v>420000000</v>
       </c>
       <c r="D52">
@@ -2406,14 +2427,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="4">
         <v>8000000</v>
       </c>
       <c r="D53">
@@ -2423,14 +2444,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
         <v>59</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="4">
         <v>350000000</v>
       </c>
       <c r="D54">
@@ -2440,14 +2461,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="4">
         <v>15000000</v>
       </c>
       <c r="D55">
@@ -2457,14 +2478,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="4">
         <v>270000000</v>
       </c>
       <c r="D56">
@@ -2474,14 +2495,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="4">
         <v>350000000</v>
       </c>
       <c r="D57">
@@ -2491,14 +2512,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" t="s">
         <v>63</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="4">
         <v>250000000</v>
       </c>
       <c r="D58">
@@ -2508,14 +2529,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>64</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="4">
         <v>150000000</v>
       </c>
       <c r="D59">
@@ -2525,14 +2546,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" t="s">
         <v>65</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="4">
         <v>90000000</v>
       </c>
       <c r="D60">
@@ -2542,14 +2563,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" t="s">
         <v>66</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="4">
         <v>350000000</v>
       </c>
       <c r="D61">
@@ -2559,14 +2580,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" t="s">
         <v>67</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="4">
         <v>900000000</v>
       </c>
       <c r="D62">
@@ -2576,14 +2597,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>68</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="4">
         <v>350000000</v>
       </c>
       <c r="D63">
@@ -2593,14 +2614,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="4">
         <v>350000000</v>
       </c>
       <c r="D64">
@@ -2610,15 +2631,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>71</v>
+      <c r="C65" s="1">
+        <v>0</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2626,15 +2647,18 @@
       <c r="E65" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F65" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="4">
         <v>70000000</v>
       </c>
       <c r="D66">
@@ -2644,14 +2668,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="4">
         <v>65000000</v>
       </c>
       <c r="D67">
@@ -2661,11 +2685,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68" s="4">
         <v>300000000</v>
       </c>
       <c r="D68">
@@ -2675,14 +2699,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" t="s">
         <v>74</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="4">
         <v>300000000</v>
       </c>
       <c r="D69">
@@ -2692,14 +2716,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70" t="s">
         <v>75</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70" s="4">
         <v>60000000</v>
       </c>
       <c r="D70">
@@ -2709,14 +2733,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="B71" t="s">
         <v>76</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71" s="4">
         <v>55000000</v>
       </c>
       <c r="D71">
@@ -2726,14 +2750,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" t="s">
         <v>77</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72" s="4">
         <v>1000000000</v>
       </c>
       <c r="D72">
@@ -2743,14 +2767,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73" t="s">
         <v>78</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73" s="4">
         <v>80000000</v>
       </c>
       <c r="D73">
@@ -2760,14 +2784,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74" s="4">
         <v>350000000</v>
       </c>
       <c r="D74">
@@ -2777,14 +2801,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75" t="s">
         <v>80</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="4">
         <v>160000000</v>
       </c>
       <c r="D75">
@@ -2794,14 +2818,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="B76" t="s">
         <v>81</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="4">
         <v>250000000</v>
       </c>
       <c r="D76">
@@ -2811,14 +2835,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="B77" t="s">
         <v>82</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="4">
         <v>330000000</v>
       </c>
       <c r="D77">
@@ -2828,14 +2852,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="B78" t="s">
         <v>83</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="4">
         <v>300000000</v>
       </c>
       <c r="D78">
@@ -2845,14 +2869,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="B79" t="s">
         <v>84</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79" s="4">
         <v>58000000</v>
       </c>
       <c r="D79">
@@ -2862,14 +2886,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
       <c r="B80" t="s">
         <v>85</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80" s="4">
         <v>95000000</v>
       </c>
       <c r="D80">
@@ -2879,14 +2903,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="B81" t="s">
         <v>86</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="4">
         <v>160000000</v>
       </c>
       <c r="D81">
@@ -2896,14 +2920,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82" t="s">
         <v>87</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="4">
         <v>75000000</v>
       </c>
       <c r="D82">
@@ -2913,14 +2937,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="B83" t="s">
         <v>88</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83" s="4">
         <v>250000000</v>
       </c>
       <c r="D83">
@@ -2930,14 +2954,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="B84" t="s">
         <v>89</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C84" s="4">
         <v>220000000</v>
       </c>
       <c r="D84">
@@ -2947,14 +2971,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
       <c r="B85" t="s">
         <v>90</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85" s="4">
         <v>500000000</v>
       </c>
       <c r="D85">
@@ -2964,14 +2988,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="B86" t="s">
         <v>91</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86" s="4">
         <v>380000000</v>
       </c>
       <c r="D86">
@@ -2981,14 +3005,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="B87" t="s">
         <v>92</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="4">
         <v>212130000</v>
       </c>
       <c r="D87">
@@ -2998,14 +3022,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
       <c r="B88" t="s">
         <v>93</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88" s="4">
         <v>250000000</v>
       </c>
       <c r="D88">
@@ -3015,14 +3039,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
       <c r="B89" t="s">
         <v>94</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C89" s="4">
         <v>565680</v>
       </c>
       <c r="D89">
@@ -3032,14 +3056,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" t="s">
         <v>95</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C90" s="4">
         <v>85000000</v>
       </c>
       <c r="D90">
@@ -3049,14 +3073,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
       <c r="B91" t="s">
         <v>96</v>
       </c>
-      <c r="C91" s="1">
+      <c r="C91" s="4">
         <v>210000000</v>
       </c>
       <c r="D91">
@@ -3066,14 +3090,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
       <c r="B92" t="s">
         <v>30</v>
       </c>
-      <c r="C92" s="1">
+      <c r="C92" s="4">
         <v>90000000</v>
       </c>
       <c r="D92">
@@ -3083,14 +3107,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
       <c r="B93" t="s">
         <v>97</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C93" s="4">
         <v>300000000</v>
       </c>
       <c r="D93">
@@ -3100,14 +3124,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
       <c r="B94" t="s">
         <v>98</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="4">
         <v>350000000</v>
       </c>
       <c r="D94">
@@ -3117,14 +3141,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95" t="s">
         <v>99</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C95" s="4">
         <v>180000000</v>
       </c>
       <c r="D95">
@@ -3134,14 +3158,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
       <c r="B96" t="s">
         <v>100</v>
       </c>
-      <c r="C96" s="1">
+      <c r="C96" s="4">
         <v>250000000</v>
       </c>
       <c r="D96">
@@ -3151,14 +3175,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="B97" t="s">
         <v>101</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="4">
         <v>250000000</v>
       </c>
       <c r="D97">
@@ -3168,14 +3192,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
       <c r="B98" t="s">
         <v>102</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="4">
         <v>300000000</v>
       </c>
       <c r="D98">
@@ -3185,14 +3209,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
       <c r="B99" t="s">
         <v>103</v>
       </c>
-      <c r="C99" s="1">
+      <c r="C99" s="4">
         <v>250000000</v>
       </c>
       <c r="D99">
@@ -3202,14 +3226,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
       <c r="B100" t="s">
         <v>104</v>
       </c>
-      <c r="C100" s="1">
+      <c r="C100" s="4">
         <v>150000000</v>
       </c>
       <c r="D100">
@@ -3219,14 +3243,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>
       <c r="B101" t="s">
         <v>105</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="4">
         <v>130000000</v>
       </c>
       <c r="D101">
@@ -3236,14 +3260,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
       <c r="B102" t="s">
         <v>106</v>
       </c>
-      <c r="C102" s="1">
+      <c r="C102" s="4">
         <v>230000000</v>
       </c>
       <c r="D102">
@@ -3253,14 +3277,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>101</v>
       </c>
       <c r="B103" t="s">
         <v>107</v>
       </c>
-      <c r="C103" s="1">
+      <c r="C103" s="4">
         <v>250000000</v>
       </c>
       <c r="D103">
@@ -3270,14 +3294,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>102</v>
       </c>
       <c r="B104" t="s">
         <v>108</v>
       </c>
-      <c r="C104" s="1">
+      <c r="C104" s="4">
         <v>350000000</v>
       </c>
       <c r="D104">
@@ -3287,14 +3311,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103</v>
       </c>
       <c r="B105" t="s">
         <v>109</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="4">
         <v>400000000</v>
       </c>
       <c r="D105">
@@ -3304,14 +3328,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>104</v>
       </c>
       <c r="B106" t="s">
         <v>110</v>
       </c>
-      <c r="C106" s="1">
+      <c r="C106" s="4">
         <v>250000000</v>
       </c>
       <c r="D106">
@@ -3321,14 +3345,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>105</v>
       </c>
       <c r="B107" t="s">
         <v>111</v>
       </c>
-      <c r="C107" s="1">
+      <c r="C107" s="4">
         <v>140000000</v>
       </c>
       <c r="D107">
@@ -3338,14 +3362,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>106</v>
       </c>
       <c r="B108" t="s">
         <v>112</v>
       </c>
-      <c r="C108" s="1">
+      <c r="C108" s="4">
         <v>250000000</v>
       </c>
       <c r="D108">
@@ -3355,14 +3379,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107</v>
       </c>
       <c r="B109" t="s">
         <v>113</v>
       </c>
-      <c r="C109" s="1">
+      <c r="C109" s="4">
         <v>65000000</v>
       </c>
       <c r="D109">
@@ -3372,14 +3396,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>108</v>
       </c>
       <c r="B110" t="s">
         <v>114</v>
       </c>
-      <c r="C110" s="1">
+      <c r="C110" s="4">
         <v>90000000</v>
       </c>
       <c r="D110">
@@ -3389,14 +3413,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>109</v>
       </c>
       <c r="B111" t="s">
         <v>115</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="4">
         <v>1131408000</v>
       </c>
       <c r="D111">
@@ -3406,14 +3430,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>110</v>
       </c>
       <c r="B112" t="s">
         <v>116</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="4">
         <v>600000</v>
       </c>
       <c r="D112">
@@ -3423,14 +3447,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>111</v>
       </c>
       <c r="B113" t="s">
         <v>117</v>
       </c>
-      <c r="C113" s="1">
+      <c r="C113" s="4">
         <v>15000000</v>
       </c>
       <c r="D113">
@@ -3440,14 +3464,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>112</v>
       </c>
       <c r="B114" t="s">
         <v>118</v>
       </c>
-      <c r="C114" s="1">
+      <c r="C114" s="4">
         <v>90000000</v>
       </c>
       <c r="D114">
@@ -3457,11 +3481,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>113</v>
       </c>
-      <c r="C115" s="1">
+      <c r="C115" s="4">
         <v>466705000</v>
       </c>
       <c r="D115">
@@ -3471,14 +3495,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>114</v>
       </c>
       <c r="B116" t="s">
         <v>119</v>
       </c>
-      <c r="C116" s="1">
+      <c r="C116" s="4">
         <v>320000000</v>
       </c>
       <c r="D116">
@@ -3488,14 +3512,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>115</v>
       </c>
       <c r="B117" t="s">
         <v>120</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="4">
         <v>37000000</v>
       </c>
       <c r="D117">
@@ -3505,14 +3529,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>116</v>
       </c>
       <c r="B118" t="s">
         <v>121</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="4">
         <v>466705000</v>
       </c>
       <c r="D118">
@@ -3522,14 +3546,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>117</v>
       </c>
       <c r="B119" t="s">
         <v>122</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="4">
         <v>212139000</v>
       </c>
       <c r="D119">
@@ -3539,14 +3563,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>118</v>
       </c>
       <c r="B120" t="s">
         <v>123</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="4">
         <v>80000000</v>
       </c>
       <c r="D120">
@@ -3556,14 +3580,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>119</v>
       </c>
       <c r="B121" t="s">
         <v>124</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="4">
         <v>120000000</v>
       </c>
       <c r="D121">
@@ -3573,14 +3597,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>120</v>
       </c>
       <c r="B122" t="s">
         <v>125</v>
       </c>
-      <c r="C122" s="1">
+      <c r="C122" s="4">
         <v>300000000</v>
       </c>
       <c r="D122">
@@ -3590,14 +3614,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>121</v>
       </c>
       <c r="B123" t="s">
         <v>126</v>
       </c>
-      <c r="C123" s="1">
+      <c r="C123" s="4">
         <v>320000000</v>
       </c>
       <c r="D123">
@@ -3607,14 +3631,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>122</v>
       </c>
       <c r="B124" t="s">
         <v>127</v>
       </c>
-      <c r="C124" s="1">
+      <c r="C124" s="4">
         <v>130000000</v>
       </c>
       <c r="D124">
@@ -3624,14 +3648,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>123</v>
       </c>
       <c r="B125" t="s">
         <v>102</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="4">
         <v>165000000</v>
       </c>
       <c r="D125">
@@ -3641,14 +3665,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>124</v>
       </c>
       <c r="B126" t="s">
         <v>82</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="4">
         <v>420000000</v>
       </c>
       <c r="D126">
@@ -3658,14 +3682,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>125</v>
       </c>
       <c r="B127" t="s">
         <v>128</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="4">
         <v>150000000</v>
       </c>
       <c r="D127">
@@ -3675,14 +3699,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>126</v>
       </c>
       <c r="B128" t="s">
         <v>129</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="4">
         <v>300000000</v>
       </c>
       <c r="D128">
@@ -3692,14 +3716,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>127</v>
       </c>
       <c r="B129" t="s">
         <v>130</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="4">
         <v>260000000</v>
       </c>
       <c r="D129">
@@ -3709,14 +3733,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>128</v>
       </c>
       <c r="B130" t="s">
         <v>131</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="4">
         <v>130000000</v>
       </c>
       <c r="D130">
@@ -3726,14 +3750,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>129</v>
       </c>
       <c r="B131" t="s">
         <v>132</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="4">
         <v>63641.7</v>
       </c>
       <c r="D131">
@@ -3743,14 +3767,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>130</v>
       </c>
       <c r="B132" t="s">
         <v>133</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="4">
         <v>800000000</v>
       </c>
       <c r="D132">
@@ -3760,14 +3784,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>131</v>
       </c>
       <c r="B133" t="s">
         <v>134</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="4">
         <v>250000000</v>
       </c>
       <c r="D133">
@@ -3777,14 +3801,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>132</v>
       </c>
       <c r="B134" t="s">
         <v>135</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="4">
         <v>212139000</v>
       </c>
       <c r="D134">
@@ -3794,14 +3818,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>133</v>
       </c>
       <c r="B135" t="s">
         <v>136</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="4">
         <v>212139000</v>
       </c>
       <c r="D135">
@@ -3811,14 +3835,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>134</v>
       </c>
       <c r="B136" t="s">
         <v>137</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="4">
         <v>1000000000</v>
       </c>
       <c r="D136">
@@ -3828,14 +3852,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>135</v>
       </c>
       <c r="B137" t="s">
         <v>138</v>
       </c>
-      <c r="C137" s="1">
+      <c r="C137" s="4">
         <v>360000000</v>
       </c>
       <c r="D137">
@@ -3845,14 +3869,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>136</v>
       </c>
       <c r="B138" t="s">
         <v>139</v>
       </c>
-      <c r="C138" s="1">
+      <c r="C138" s="4">
         <v>707130000</v>
       </c>
       <c r="D138">
@@ -3862,14 +3886,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>137</v>
       </c>
       <c r="B139" t="s">
         <v>140</v>
       </c>
-      <c r="C139" s="1">
+      <c r="C139" s="4">
         <v>50000000</v>
       </c>
       <c r="D139">
@@ -3879,14 +3903,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>138</v>
       </c>
       <c r="B140" t="s">
         <v>141</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="4">
         <v>300000000</v>
       </c>
       <c r="D140">
@@ -3896,14 +3920,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>139</v>
       </c>
       <c r="B141" t="s">
         <v>142</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="4">
         <v>200000000</v>
       </c>
       <c r="D141">
@@ -3913,14 +3937,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>140</v>
       </c>
       <c r="B142" t="s">
         <v>143</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="4">
         <v>170000000</v>
       </c>
       <c r="D142">
@@ -3930,14 +3954,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>141</v>
       </c>
       <c r="B143" t="s">
         <v>144</v>
       </c>
-      <c r="C143" s="1">
+      <c r="C143" s="4">
         <v>100000000</v>
       </c>
       <c r="D143">
@@ -3947,14 +3971,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>142</v>
       </c>
       <c r="B144" t="s">
         <v>145</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="4">
         <v>200000000</v>
       </c>
       <c r="D144">
@@ -3964,14 +3988,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>143</v>
       </c>
       <c r="B145" t="s">
         <v>146</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="4">
         <v>850000000</v>
       </c>
       <c r="D145">
@@ -3981,14 +4005,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>144</v>
       </c>
       <c r="B146" t="s">
         <v>147</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="4">
         <v>210000000</v>
       </c>
       <c r="D146">
@@ -3998,14 +4022,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>145</v>
       </c>
       <c r="B147" t="s">
         <v>148</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="4">
         <v>210000000</v>
       </c>
       <c r="D147">
@@ -4015,14 +4039,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>146</v>
       </c>
       <c r="B148" t="s">
         <v>149</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="4">
         <v>30000000</v>
       </c>
       <c r="D148">
@@ -4032,14 +4056,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>147</v>
       </c>
       <c r="B149" t="s">
         <v>150</v>
       </c>
-      <c r="C149" s="1">
+      <c r="C149" s="4">
         <v>400000000</v>
       </c>
       <c r="D149">
@@ -4049,14 +4073,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>148</v>
       </c>
       <c r="B150" t="s">
         <v>151</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="4">
         <v>169711000</v>
       </c>
       <c r="D150">
@@ -4066,14 +4090,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>149</v>
       </c>
       <c r="B151" t="s">
         <v>152</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="4">
         <v>260000000</v>
       </c>
       <c r="D151">
@@ -4083,14 +4107,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>150</v>
       </c>
       <c r="B152" t="s">
         <v>153</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="4">
         <v>271537920</v>
       </c>
       <c r="D152">
@@ -4100,14 +4124,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>151</v>
       </c>
       <c r="B153" t="s">
         <v>154</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="4">
         <v>320000000</v>
       </c>
       <c r="D153">
@@ -4117,14 +4141,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>152</v>
       </c>
       <c r="B154" t="s">
         <v>155</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="4">
         <v>200000000</v>
       </c>
       <c r="D154">
@@ -4134,14 +4158,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>153</v>
       </c>
       <c r="B155" t="s">
         <v>156</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="4">
         <v>130000000</v>
       </c>
       <c r="D155">
@@ -4151,14 +4175,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>154</v>
       </c>
       <c r="B156" t="s">
         <v>150</v>
       </c>
-      <c r="C156" s="1">
+      <c r="C156" s="4">
         <v>210000000</v>
       </c>
       <c r="D156">
@@ -4168,14 +4192,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>155</v>
       </c>
       <c r="B157" t="s">
         <v>157</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="4">
         <v>150000000</v>
       </c>
       <c r="D157">
@@ -4185,14 +4209,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>156</v>
       </c>
       <c r="B158" t="s">
         <v>158</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="4">
         <v>175000000</v>
       </c>
       <c r="D158">
@@ -4202,14 +4226,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>157</v>
       </c>
       <c r="B159" t="s">
         <v>159</v>
       </c>
-      <c r="C159" s="1">
+      <c r="C159" s="4">
         <v>282852000</v>
       </c>
       <c r="D159">
@@ -4219,14 +4243,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>158</v>
       </c>
       <c r="B160" t="s">
         <v>160</v>
       </c>
-      <c r="C160" s="1">
+      <c r="C160" s="4">
         <v>175000000</v>
       </c>
       <c r="D160">
@@ -4236,14 +4260,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>159</v>
       </c>
       <c r="B161" t="s">
         <v>161</v>
       </c>
-      <c r="C161" s="1">
+      <c r="C161" s="4">
         <v>68000000</v>
       </c>
       <c r="D161">
@@ -4253,14 +4277,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>160</v>
       </c>
       <c r="B162" t="s">
         <v>162</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="4">
         <v>150000000</v>
       </c>
       <c r="D162">
@@ -4270,14 +4294,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>161</v>
       </c>
       <c r="B163" t="s">
         <v>163</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="4">
         <v>60000000</v>
       </c>
       <c r="D163">
@@ -4287,14 +4311,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>162</v>
       </c>
       <c r="B164" t="s">
         <v>164</v>
       </c>
-      <c r="C164" s="1">
+      <c r="C164" s="4">
         <v>250000000</v>
       </c>
       <c r="D164">
@@ -4304,14 +4328,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>163</v>
       </c>
       <c r="B165" t="s">
         <v>102</v>
       </c>
-      <c r="C165" s="1">
+      <c r="C165" s="4">
         <v>200000000</v>
       </c>
       <c r="D165">
@@ -4321,14 +4345,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>164</v>
       </c>
       <c r="B166" t="s">
         <v>102</v>
       </c>
-      <c r="C166" s="1">
+      <c r="C166" s="4">
         <v>200000000</v>
       </c>
       <c r="D166">
@@ -4338,14 +4362,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>165</v>
       </c>
       <c r="B167" t="s">
         <v>165</v>
       </c>
-      <c r="C167" s="1">
+      <c r="C167" s="4">
         <v>707130000</v>
       </c>
       <c r="D167">
@@ -4355,14 +4379,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>166</v>
       </c>
       <c r="B168" t="s">
         <v>166</v>
       </c>
-      <c r="C168" s="1">
+      <c r="C168" s="4">
         <v>250000000</v>
       </c>
       <c r="D168">
@@ -4372,14 +4396,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>167</v>
       </c>
       <c r="B169" t="s">
         <v>167</v>
       </c>
-      <c r="C169" s="1">
+      <c r="C169" s="4">
         <v>350000000</v>
       </c>
       <c r="D169">
@@ -4389,14 +4413,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>168</v>
       </c>
       <c r="B170" t="s">
         <v>168</v>
       </c>
-      <c r="C170" s="1">
+      <c r="C170" s="4">
         <v>300000000</v>
       </c>
       <c r="D170">
@@ -4406,14 +4430,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>169</v>
       </c>
       <c r="B171" t="s">
         <v>169</v>
       </c>
-      <c r="C171" s="1">
+      <c r="C171" s="4">
         <v>350000000</v>
       </c>
       <c r="D171">
@@ -4423,14 +4447,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>170</v>
       </c>
       <c r="B172" t="s">
         <v>170</v>
       </c>
-      <c r="C172" s="1">
+      <c r="C172" s="4">
         <v>220000000</v>
       </c>
       <c r="D172">
@@ -4440,14 +4464,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>171</v>
       </c>
       <c r="B173" t="s">
         <v>102</v>
       </c>
-      <c r="C173" s="1">
+      <c r="C173" s="4">
         <v>150000000</v>
       </c>
       <c r="D173">
@@ -4457,14 +4481,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>172</v>
       </c>
       <c r="B174" t="s">
         <v>171</v>
       </c>
-      <c r="C174" s="1">
+      <c r="C174" s="4">
         <v>35000000</v>
       </c>
       <c r="D174">
@@ -4474,14 +4498,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>173</v>
       </c>
       <c r="B175" t="s">
         <v>172</v>
       </c>
-      <c r="C175" s="1">
+      <c r="C175" s="4">
         <v>127283400</v>
       </c>
       <c r="D175">
@@ -4491,14 +4515,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>174</v>
       </c>
       <c r="B176" t="s">
         <v>173</v>
       </c>
-      <c r="C176" s="1">
+      <c r="C176" s="4">
         <v>75000000</v>
       </c>
       <c r="D176">
@@ -4508,14 +4532,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>175</v>
       </c>
       <c r="B177" t="s">
         <v>174</v>
       </c>
-      <c r="C177" s="1">
+      <c r="C177" s="4">
         <v>45000000</v>
       </c>
       <c r="D177">
@@ -4525,14 +4549,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>176</v>
       </c>
       <c r="B178" t="s">
         <v>175</v>
       </c>
-      <c r="C178" s="1">
+      <c r="C178" s="4">
         <v>250000000</v>
       </c>
       <c r="D178">
@@ -4542,14 +4566,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>177</v>
       </c>
       <c r="B179" t="s">
         <v>176</v>
       </c>
-      <c r="C179" s="1">
+      <c r="C179" s="4">
         <v>120000000</v>
       </c>
       <c r="D179">
@@ -4559,14 +4583,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>178</v>
       </c>
       <c r="B180" t="s">
         <v>177</v>
       </c>
-      <c r="C180" s="1">
+      <c r="C180" s="4">
         <v>180000000</v>
       </c>
       <c r="D180">
@@ -4576,14 +4600,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>179</v>
       </c>
       <c r="B181" t="s">
         <v>178</v>
       </c>
-      <c r="C181" s="1">
+      <c r="C181" s="4">
         <v>300000000</v>
       </c>
       <c r="D181">
@@ -4593,14 +4617,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>180</v>
       </c>
       <c r="B182" t="s">
         <v>102</v>
       </c>
-      <c r="C182" s="1">
+      <c r="C182" s="4">
         <v>300000000</v>
       </c>
       <c r="D182">
@@ -4610,14 +4634,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>181</v>
       </c>
       <c r="B183" t="s">
         <v>179</v>
       </c>
-      <c r="C183" s="1">
+      <c r="C183" s="4">
         <v>160000000</v>
       </c>
       <c r="D183">
@@ -4627,14 +4651,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>182</v>
       </c>
       <c r="B184" t="s">
         <v>180</v>
       </c>
-      <c r="C184" s="1">
+      <c r="C184" s="4">
         <v>200000000</v>
       </c>
       <c r="D184">
@@ -4644,14 +4668,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>183</v>
       </c>
       <c r="B185" t="s">
         <v>181</v>
       </c>
-      <c r="C185" s="1">
+      <c r="C185" s="4">
         <v>160000000</v>
       </c>
       <c r="D185">
@@ -4661,14 +4685,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>184</v>
       </c>
       <c r="B186" t="s">
         <v>182</v>
       </c>
-      <c r="C186" s="1">
+      <c r="C186" s="4">
         <v>3339422400</v>
       </c>
       <c r="D186">
@@ -4678,14 +4702,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>185</v>
       </c>
       <c r="B187" t="s">
         <v>82</v>
       </c>
-      <c r="C187" s="1">
+      <c r="C187" s="4">
         <v>200000000</v>
       </c>
       <c r="D187">
@@ -4695,14 +4719,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>186</v>
       </c>
       <c r="B188" t="s">
         <v>183</v>
       </c>
-      <c r="C188" s="1">
+      <c r="C188" s="4">
         <v>150000000</v>
       </c>
       <c r="D188">
@@ -4712,14 +4736,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>187</v>
       </c>
       <c r="B189" t="s">
         <v>184</v>
       </c>
-      <c r="C189" s="1">
+      <c r="C189" s="4">
         <v>200000000</v>
       </c>
       <c r="D189">
@@ -4729,14 +4753,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>188</v>
       </c>
       <c r="B190" t="s">
         <v>185</v>
       </c>
-      <c r="C190" s="1">
+      <c r="C190" s="4">
         <v>270000000</v>
       </c>
       <c r="D190">
@@ -4746,14 +4770,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>189</v>
       </c>
       <c r="B191" t="s">
         <v>186</v>
       </c>
-      <c r="C191" s="1">
+      <c r="C191" s="4">
         <v>180000000</v>
       </c>
       <c r="D191">
@@ -4763,14 +4787,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>190</v>
       </c>
       <c r="B192" t="s">
         <v>187</v>
       </c>
-      <c r="C192" s="1">
+      <c r="C192" s="4">
         <v>1000000</v>
       </c>
       <c r="D192">
@@ -4780,14 +4804,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>191</v>
       </c>
       <c r="B193" t="s">
         <v>188</v>
       </c>
-      <c r="C193" s="1">
+      <c r="C193" s="4">
         <v>180000000</v>
       </c>
       <c r="D193">
@@ -4797,14 +4821,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>192</v>
       </c>
       <c r="B194" t="s">
         <v>189</v>
       </c>
-      <c r="C194" s="1">
+      <c r="C194" s="4">
         <v>100000000</v>
       </c>
       <c r="D194">
@@ -4814,14 +4838,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>193</v>
       </c>
       <c r="B195" t="s">
         <v>190</v>
       </c>
-      <c r="C195" s="1">
+      <c r="C195" s="4">
         <v>100000000</v>
       </c>
       <c r="D195">
@@ -4831,14 +4855,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>194</v>
       </c>
       <c r="B196" t="s">
         <v>191</v>
       </c>
-      <c r="C196" s="1">
+      <c r="C196" s="4">
         <v>160000000</v>
       </c>
       <c r="D196">
@@ -4848,14 +4872,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>195</v>
       </c>
       <c r="B197" t="s">
         <v>192</v>
       </c>
-      <c r="C197" s="1">
+      <c r="C197" s="4">
         <v>600000000</v>
       </c>
       <c r="D197">
@@ -4865,14 +4889,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>196</v>
       </c>
       <c r="B198" t="s">
         <v>193</v>
       </c>
-      <c r="C198" s="1">
+      <c r="C198" s="4">
         <v>15000000</v>
       </c>
       <c r="D198">
@@ -4882,14 +4906,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>197</v>
       </c>
       <c r="B199" t="s">
         <v>194</v>
       </c>
-      <c r="C199" s="1">
+      <c r="C199" s="4">
         <v>47000000</v>
       </c>
       <c r="D199">
@@ -4899,14 +4923,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>198</v>
       </c>
       <c r="B200" t="s">
         <v>195</v>
       </c>
-      <c r="C200" s="1">
+      <c r="C200" s="4">
         <v>200000000</v>
       </c>
       <c r="D200">
@@ -4916,14 +4940,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>199</v>
       </c>
       <c r="B201" t="s">
         <v>31</v>
       </c>
-      <c r="C201" s="1">
+      <c r="C201" s="4">
         <v>185000000</v>
       </c>
       <c r="D201">
@@ -4933,14 +4957,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>200</v>
       </c>
       <c r="B202" t="s">
         <v>196</v>
       </c>
-      <c r="C202" s="1">
+      <c r="C202" s="4">
         <v>250000000</v>
       </c>
       <c r="D202">
@@ -4950,14 +4974,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>201</v>
       </c>
       <c r="B203" t="s">
         <v>197</v>
       </c>
-      <c r="C203" s="1">
+      <c r="C203" s="4">
         <v>200000000</v>
       </c>
       <c r="D203">
@@ -4967,14 +4991,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>202</v>
       </c>
       <c r="B204" t="s">
         <v>198</v>
       </c>
-      <c r="C204" s="1">
+      <c r="C204" s="4">
         <v>200000000</v>
       </c>
       <c r="D204">
@@ -4984,14 +5008,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>203</v>
       </c>
       <c r="B205" t="s">
         <v>199</v>
       </c>
-      <c r="C205" s="1">
+      <c r="C205" s="4">
         <v>270000000</v>
       </c>
       <c r="D205">
@@ -5001,14 +5025,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>204</v>
       </c>
       <c r="B206" t="s">
         <v>201</v>
       </c>
-      <c r="C206" s="1">
+      <c r="C206" s="4">
         <v>848556</v>
       </c>
       <c r="D206">
@@ -5018,14 +5042,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>205</v>
       </c>
       <c r="B207" t="s">
         <v>202</v>
       </c>
-      <c r="C207" s="1">
+      <c r="C207" s="4">
         <v>20000000</v>
       </c>
       <c r="D207">
@@ -5035,14 +5059,14 @@
         <v>203</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>206</v>
       </c>
       <c r="B208" t="s">
         <v>204</v>
       </c>
-      <c r="C208" s="1">
+      <c r="C208" s="4">
         <v>141426000</v>
       </c>
       <c r="D208">
@@ -5052,14 +5076,14 @@
         <v>203</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>207</v>
       </c>
       <c r="B209" t="s">
         <v>205</v>
       </c>
-      <c r="C209" s="1">
+      <c r="C209" s="4">
         <v>160000000</v>
       </c>
       <c r="D209">
@@ -5069,14 +5093,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>208</v>
       </c>
       <c r="B210" t="s">
         <v>206</v>
       </c>
-      <c r="C210" s="1">
+      <c r="C210" s="4">
         <v>169711200</v>
       </c>
       <c r="D210">
@@ -5086,14 +5110,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>209</v>
       </c>
       <c r="B211" t="s">
         <v>207</v>
       </c>
-      <c r="C211" s="1">
+      <c r="C211" s="4">
         <v>848556</v>
       </c>
       <c r="D211">
@@ -5103,14 +5127,14 @@
         <v>208</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>210</v>
       </c>
       <c r="B212" t="s">
         <v>209</v>
       </c>
-      <c r="C212" s="1">
+      <c r="C212" s="4">
         <v>230000000</v>
       </c>
       <c r="D212">
@@ -5120,14 +5144,14 @@
         <v>203</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>211</v>
       </c>
       <c r="B213" t="s">
         <v>210</v>
       </c>
-      <c r="C213" s="1">
+      <c r="C213" s="4">
         <v>1000000</v>
       </c>
       <c r="D213">
@@ -5137,15 +5161,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>212</v>
       </c>
       <c r="B214" t="s">
         <v>211</v>
       </c>
-      <c r="C214" s="1" t="s">
-        <v>222</v>
+      <c r="C214" s="4">
+        <v>2121390</v>
       </c>
       <c r="D214">
         <v>0</v>
@@ -5154,14 +5178,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>213</v>
       </c>
       <c r="B215" t="s">
         <v>212</v>
       </c>
-      <c r="C215" s="1">
+      <c r="C215" s="4">
         <v>40000</v>
       </c>
       <c r="D215">
@@ -5171,14 +5195,14 @@
         <v>203</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>214</v>
       </c>
       <c r="B216" t="s">
         <v>213</v>
       </c>
-      <c r="C216" s="1">
+      <c r="C216" s="4">
         <v>120212000</v>
       </c>
       <c r="D216">
@@ -5188,14 +5212,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>215</v>
       </c>
       <c r="B217" t="s">
         <v>214</v>
       </c>
-      <c r="C217" s="1">
+      <c r="C217" s="4">
         <v>95000000</v>
       </c>
       <c r="D217">
@@ -5205,14 +5229,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>216</v>
       </c>
       <c r="B218" t="s">
         <v>215</v>
       </c>
-      <c r="C218" s="1">
+      <c r="C218" s="4">
         <v>919269000</v>
       </c>
       <c r="D218">
@@ -5222,14 +5246,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>217</v>
       </c>
       <c r="B219" t="s">
         <v>216</v>
       </c>
-      <c r="C219" s="1">
+      <c r="C219" s="4">
         <v>40000000</v>
       </c>
       <c r="D219">
@@ -5239,14 +5263,14 @@
         <v>203</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>218</v>
       </c>
       <c r="B220" t="s">
         <v>217</v>
       </c>
-      <c r="C220" s="1">
+      <c r="C220" s="4">
         <v>150000000</v>
       </c>
       <c r="D220">
@@ -5256,14 +5280,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>219</v>
       </c>
       <c r="B221" t="s">
         <v>218</v>
       </c>
-      <c r="C221" s="1">
+      <c r="C221" s="4">
         <v>282852000</v>
       </c>
       <c r="D221">
@@ -5273,14 +5297,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>220</v>
       </c>
       <c r="B222" t="s">
         <v>127</v>
       </c>
-      <c r="C222" s="1">
+      <c r="C222" s="4">
         <v>62000000</v>
       </c>
       <c r="D222">
@@ -5290,14 +5314,14 @@
         <v>219</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>221</v>
       </c>
       <c r="B223" t="s">
         <v>220</v>
       </c>
-      <c r="C223" s="1">
+      <c r="C223" s="4">
         <v>134354700</v>
       </c>
       <c r="D223">
@@ -5307,14 +5331,14 @@
         <v>219</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>222</v>
       </c>
       <c r="B224" t="s">
         <v>221</v>
       </c>
-      <c r="C224" s="1">
+      <c r="C224" s="4">
         <v>127283400</v>
       </c>
       <c r="D224">
@@ -5324,7 +5348,11 @@
         <v>219</v>
       </c>
     </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C225" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>